<commit_message>
After re-arrange Test Object
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="123">
   <si>
     <t>ID:</t>
   </si>
@@ -191,96 +191,6 @@
     <t>katalonhunguser0020</t>
   </si>
   <si>
-    <t>katalonhunguser0021</t>
-  </si>
-  <si>
-    <t>katalonhunguser0022</t>
-  </si>
-  <si>
-    <t>katalonhunguser0023</t>
-  </si>
-  <si>
-    <t>katalonhunguser0024</t>
-  </si>
-  <si>
-    <t>katalonhunguser0025</t>
-  </si>
-  <si>
-    <t>katalonhunguser0026</t>
-  </si>
-  <si>
-    <t>katalonhunguser0027</t>
-  </si>
-  <si>
-    <t>katalonhunguser0028</t>
-  </si>
-  <si>
-    <t>katalonhunguser0029</t>
-  </si>
-  <si>
-    <t>katalonhunguser0030</t>
-  </si>
-  <si>
-    <t>katalonhunguser0031</t>
-  </si>
-  <si>
-    <t>katalonhunguser0032</t>
-  </si>
-  <si>
-    <t>katalonhunguser0033</t>
-  </si>
-  <si>
-    <t>katalonhunguser0034</t>
-  </si>
-  <si>
-    <t>katalonhunguser0035</t>
-  </si>
-  <si>
-    <t>katalonhunguser0036</t>
-  </si>
-  <si>
-    <t>katalonhunguser0037</t>
-  </si>
-  <si>
-    <t>katalonhunguser0038</t>
-  </si>
-  <si>
-    <t>katalonhunguser0039</t>
-  </si>
-  <si>
-    <t>katalonhunguser0040</t>
-  </si>
-  <si>
-    <t>katalonhunguser0041</t>
-  </si>
-  <si>
-    <t>katalonhunguser0042</t>
-  </si>
-  <si>
-    <t>katalonhunguser0043</t>
-  </si>
-  <si>
-    <t>katalonhunguser0044</t>
-  </si>
-  <si>
-    <t>katalonhunguser0045</t>
-  </si>
-  <si>
-    <t>katalonhunguser0046</t>
-  </si>
-  <si>
-    <t>katalonhunguser0047</t>
-  </si>
-  <si>
-    <t>katalonhunguser0048</t>
-  </si>
-  <si>
-    <t>katalonhunguser0049</t>
-  </si>
-  <si>
-    <t>katalonhunguser0050</t>
-  </si>
-  <si>
     <t>Hoang</t>
   </si>
   <si>
@@ -419,28 +329,67 @@
     <t>Nhi</t>
   </si>
   <si>
+    <t>kahung0001o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>kahung0002o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>locking like</t>
+  </si>
+  <si>
+    <t>kahung0003o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>kahung0004o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>Luu</t>
+  </si>
+  <si>
+    <t>Nguyet</t>
+  </si>
+  <si>
+    <t>kahung0001g@gmail.com</t>
+  </si>
+  <si>
+    <t>Yen</t>
+  </si>
+  <si>
+    <t>kahung0002g@gmail.com</t>
+  </si>
+  <si>
+    <t>Nhu</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>kahung0005o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>kahung0006o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>Hoa</t>
+  </si>
+  <si>
     <t>locking</t>
   </si>
   <si>
-    <t>kahung0001o@outlook.com.vn</t>
-  </si>
-  <si>
-    <t>kahung0002o@outlook.com.vn</t>
-  </si>
-  <si>
-    <t>locking like</t>
-  </si>
-  <si>
-    <t>kahung0003o@outlook.com.vn</t>
-  </si>
-  <si>
-    <t>kahung0004o@outlook.com.vn</t>
-  </si>
-  <si>
-    <t>Luu</t>
-  </si>
-  <si>
-    <t>Nguyet</t>
+    <t>kahung0007o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>kahung0008o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>kahung0009o@outlook.com.vn</t>
+  </si>
+  <si>
+    <t>Thao</t>
+  </si>
+  <si>
+    <t>Huynh</t>
   </si>
 </sst>
 </file>
@@ -798,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,10 +758,12 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="35.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,42 +773,51 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -868,13 +828,13 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -885,13 +845,13 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -902,13 +862,13 @@
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -919,13 +879,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -942,7 +902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -959,7 +919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -976,7 +936,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -993,7 +953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1010,7 +970,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1027,7 +987,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1044,7 +1004,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1061,7 +1021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1117,7 +1077,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>3</v>
@@ -1126,7 +1086,7 @@
         <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1134,7 +1094,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>3</v>
@@ -1151,16 +1111,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1168,36 +1128,33 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>114</v>
+      <c r="B23" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1205,16 +1162,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1222,19 +1179,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1242,13 +1199,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>26</v>
@@ -1259,13 +1216,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>26</v>
@@ -1276,7 +1233,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>3</v>
@@ -1285,7 +1242,7 @@
         <v>29</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1293,16 +1250,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1310,7 +1267,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>3</v>
@@ -1319,7 +1276,7 @@
         <v>29</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,16 +1284,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1344,16 +1301,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1361,44 +1318,41 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>133</v>
+      <c r="B34" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>134</v>
+      <c r="B35" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>3</v>
@@ -1407,7 +1361,10 @@
         <v>29</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>122</v>
+        <v>92</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1415,16 +1372,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,16 +1389,135 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>139</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1452,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,628 +1558,6 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>35</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>37</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>38</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>39</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>41</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>42</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>43</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>44</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>45</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>46</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>47</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>48</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>49</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>50</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -2152,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>